<commit_message>
Project Management Guidelines Added
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Information Technology\Software Engineering - Project\SE Project\semantic-similarity-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6DD08-3D4D-454F-8012-CE26F93A09FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E64101-1727-41C7-8465-52370DA754F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -842,7 +842,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Project Management Guidelines updated
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Information Technology\Software Engineering - Project\SE Project\semantic-similarity-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E64101-1727-41C7-8465-52370DA754F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5002F6E-A411-4A48-A61C-5481890681A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -842,7 +842,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A6" sqref="A6:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changes in Gantt Chart and program
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Information Technology\Software Engineering - Project\SE Project\semantic-similarity-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5002F6E-A411-4A48-A61C-5481890681A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B96376A-ABC2-44C3-908B-B834BCD246CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Project Start:</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Gathering information, analyzing the project, and reviewing current methods.</t>
+  </si>
+  <si>
+    <t>Achieved</t>
+  </si>
+  <si>
+    <t>Not completed in this sprint</t>
   </si>
 </sst>
 </file>
@@ -839,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -854,7 +860,7 @@
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.75" thickBot="1">
+    <row r="1" spans="1:6" ht="27.75" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
@@ -863,7 +869,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1">
       <c r="A2" s="20" t="s">
         <v>13</v>
       </c>
@@ -872,7 +878,7 @@
       <c r="D2" s="21"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
@@ -884,7 +890,7 @@
       </c>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="1:5" ht="24">
+    <row r="4" spans="1:6" ht="24">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -901,7 +907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -918,7 +924,7 @@
         <v>45741</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -932,8 +938,11 @@
       <c r="E6" s="11">
         <v>45671</v>
       </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -947,8 +956,11 @@
       <c r="E7" s="11">
         <v>45685</v>
       </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -962,8 +974,11 @@
       <c r="E8" s="11">
         <v>45699</v>
       </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
@@ -978,7 +993,7 @@
         <v>45741</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>45727</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>

</xml_diff>